<commit_message>
added the design pic
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\OneDrive\Documents\Abhishek\Stock\Alpacatrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{704C0B58-C8E6-4EDE-AD57-5B560AC8EC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA78DB1-96EC-480A-A7F3-6FE77F1FAC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-330" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{A1DBCF56-1C1C-4CEA-B61C-09CC4D5D8075}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Step 1</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Sell all and transations by 2:45 PM.</t>
+  </si>
+  <si>
+    <t>10,000-&gt;10,200   , AAPL-5000-&gt;5400 ,NKLA- etc</t>
   </si>
 </sst>
 </file>
@@ -706,7 +709,7 @@
   <dimension ref="A3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,7 +836,9 @@
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>